<commit_message>
- Tested all environments with noise
</commit_message>
<xml_diff>
--- a/src/output/opt/noise/data.xlsx
+++ b/src/output/opt/noise/data.xlsx
@@ -53,24 +53,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="true"/>
-    <col min="2" max="2" width="5.140625" customWidth="true"/>
-    <col min="3" max="3" width="2.140625" customWidth="true"/>
-    <col min="4" max="4" width="3.7109375" customWidth="true"/>
-    <col min="5" max="5" width="4.140625" customWidth="true"/>
-    <col min="6" max="6" width="4.7109375" customWidth="true"/>
-    <col min="7" max="7" width="5.140625" customWidth="true"/>
-    <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="15.7109375" customWidth="true"/>
-    <col min="10" max="10" width="16.28515625" customWidth="true"/>
-    <col min="11" max="11" width="2.140625" customWidth="true"/>
-    <col min="12" max="12" width="4.140625" customWidth="true"/>
+    <col min="1" max="1" width="3" customWidth="true"/>
+    <col min="2" max="2" width="5" customWidth="true"/>
+    <col min="3" max="3" width="2" customWidth="true"/>
+    <col min="4" max="4" width="3.5546875" customWidth="true"/>
+    <col min="5" max="5" width="3" customWidth="true"/>
+    <col min="6" max="6" width="5" customWidth="true"/>
+    <col min="7" max="7" width="3.5546875" customWidth="true"/>
+    <col min="8" max="8" width="3" customWidth="true"/>
+    <col min="9" max="9" width="5" customWidth="true"/>
+    <col min="10" max="10" width="11.5546875" customWidth="true"/>
+    <col min="11" max="11" width="15.5546875" customWidth="true"/>
+    <col min="12" max="12" width="15.88671875" customWidth="true"/>
+    <col min="13" max="13" width="2" customWidth="true"/>
+    <col min="14" max="14" width="4" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -87,27 +89,33 @@
         <v>2.5</v>
       </c>
       <c r="E1" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F1" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G1" s="0">
-        <v>1262</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H1" s="0">
-        <v>348.08444429999997</v>
+        <v>10</v>
       </c>
       <c r="I1" s="0">
-        <v>0.00015597136462863759</v>
+        <v>221</v>
       </c>
       <c r="J1" s="0">
-        <v>-1.6441482591255901e-06</v>
+        <v>37.592995899999998</v>
       </c>
       <c r="K1" s="0">
-        <v>0</v>
+        <v>6.4932694991970408e-06</v>
       </c>
       <c r="L1" s="0">
+        <v>8.0009670018521097e-08</v>
+      </c>
+      <c r="M1" s="0">
+        <v>0</v>
+      </c>
+      <c r="N1" s="0">
         <v>0</v>
       </c>
     </row>
@@ -125,28 +133,34 @@
         <v>2.5</v>
       </c>
       <c r="E2" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G2" s="0">
-        <v>312</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H2" s="0">
-        <v>89.736347600000002</v>
+        <v>10</v>
       </c>
       <c r="I2" s="0">
-        <v>6.8116042360788498e-05</v>
+        <v>269</v>
       </c>
       <c r="J2" s="0">
-        <v>6.0693372676457197e-07</v>
+        <v>93.003292599999995</v>
       </c>
       <c r="K2" s="0">
-        <v>1</v>
+        <v>7.2171191389802658e-06</v>
       </c>
       <c r="L2" s="0">
-        <v>82</v>
+        <v>6.287673443285553e-08</v>
+      </c>
+      <c r="M2" s="0">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -163,28 +177,34 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G3" s="0">
-        <v>369</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H3" s="0">
-        <v>199.23783420000001</v>
+        <v>10</v>
       </c>
       <c r="I3" s="0">
-        <v>0.00018531213506078892</v>
+        <v>269</v>
       </c>
       <c r="J3" s="0">
-        <v>-4.3988692627432443e-06</v>
+        <v>100.07330109999999</v>
       </c>
       <c r="K3" s="0">
-        <v>1</v>
+        <v>7.1573757296494733e-06</v>
       </c>
       <c r="L3" s="0">
-        <v>44</v>
+        <v>5.8150525727170281e-08</v>
+      </c>
+      <c r="M3" s="0">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -201,28 +221,34 @@
         <v>2.5</v>
       </c>
       <c r="E4" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G4" s="0">
-        <v>269</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H4" s="0">
-        <v>244.98417230000001</v>
+        <v>10</v>
       </c>
       <c r="I4" s="0">
-        <v>0.00078415626376182601</v>
+        <v>275</v>
       </c>
       <c r="J4" s="0">
-        <v>-3.0608607912803039e-05</v>
+        <v>130.79598559999999</v>
       </c>
       <c r="K4" s="0">
-        <v>2</v>
+        <v>6.4342353602864222e-06</v>
       </c>
       <c r="L4" s="0">
-        <v>175</v>
+        <v>8.4126528430352524e-08</v>
+      </c>
+      <c r="M4" s="0">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -239,28 +265,34 @@
         <v>2.5</v>
       </c>
       <c r="E5" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G5" s="0">
-        <v>269</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H5" s="0">
-        <v>245.85245330000001</v>
+        <v>10</v>
       </c>
       <c r="I5" s="0">
-        <v>0.00035683199620062389</v>
+        <v>238</v>
       </c>
       <c r="J5" s="0">
-        <v>-3.9766926691228031e-05</v>
+        <v>100.3150967</v>
       </c>
       <c r="K5" s="0">
-        <v>2</v>
+        <v>7.2719002239818309e-06</v>
       </c>
       <c r="L5" s="0">
-        <v>175</v>
+        <v>3.4547054183295656e-08</v>
+      </c>
+      <c r="M5" s="0">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0">
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -277,27 +309,517 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G6" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H6" s="0">
+        <v>10</v>
+      </c>
+      <c r="I6" s="0">
+        <v>779</v>
+      </c>
+      <c r="J6" s="0">
+        <v>420.76224239999999</v>
+      </c>
+      <c r="K6" s="0">
+        <v>7.3346758511227961e-06</v>
+      </c>
+      <c r="L6" s="0">
+        <v>1.0632717650283736e-08</v>
+      </c>
+      <c r="M6" s="0">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="0">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E7" s="0">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H7" s="0">
+        <v>10</v>
+      </c>
+      <c r="I7" s="0">
+        <v>1262</v>
+      </c>
+      <c r="J7" s="0">
+        <v>436.4591729</v>
+      </c>
+      <c r="K7" s="0">
+        <v>1.7145014564734495e-05</v>
+      </c>
+      <c r="L7" s="0">
+        <v>-1.3758434871880631e-07</v>
+      </c>
+      <c r="M7" s="0">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="0">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="0">
+        <v>10</v>
+      </c>
+      <c r="F8" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H8" s="0">
+        <v>10</v>
+      </c>
+      <c r="I8" s="0">
+        <v>285</v>
+      </c>
+      <c r="J8" s="0">
+        <v>108.8751674</v>
+      </c>
+      <c r="K8" s="0">
+        <v>7.287129319077934e-06</v>
+      </c>
+      <c r="L8" s="0">
+        <v>5.0733148107113003e-08</v>
+      </c>
+      <c r="M8" s="0">
+        <v>1</v>
+      </c>
+      <c r="N8" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E9" s="0">
+        <v>10</v>
+      </c>
+      <c r="F9" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H9" s="0">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0">
+        <v>312</v>
+      </c>
+      <c r="J9" s="0">
+        <v>119.39946329999999</v>
+      </c>
+      <c r="K9" s="0">
+        <v>2.7864391593190874e-05</v>
+      </c>
+      <c r="L9" s="0">
+        <v>3.6311749339572998e-08</v>
+      </c>
+      <c r="M9" s="0">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="0">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="0">
+        <v>10</v>
+      </c>
+      <c r="F10" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H10" s="0">
+        <v>10</v>
+      </c>
+      <c r="I10" s="0">
+        <v>369</v>
+      </c>
+      <c r="J10" s="0">
+        <v>228.01029969999999</v>
+      </c>
+      <c r="K10" s="0">
+        <v>2.7973201768949352e-05</v>
+      </c>
+      <c r="L10" s="0">
+        <v>-7.973671549211776e-07</v>
+      </c>
+      <c r="M10" s="0">
+        <v>1</v>
+      </c>
+      <c r="N10" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="0">
+        <v>5</v>
+      </c>
+      <c r="D11" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="0">
+        <v>10</v>
+      </c>
+      <c r="F11" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H11" s="0">
+        <v>10</v>
+      </c>
+      <c r="I11" s="0">
         <v>269</v>
       </c>
-      <c r="H6" s="0">
-        <v>256.17017679999998</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0.001952341701944027</v>
-      </c>
-      <c r="J6" s="0">
-        <v>-3.0092198418340354e-05</v>
-      </c>
-      <c r="K6" s="0">
+      <c r="J11" s="0">
+        <v>231.72164889999999</v>
+      </c>
+      <c r="K11" s="0">
+        <v>7.5919017148429191e-05</v>
+      </c>
+      <c r="L11" s="0">
+        <v>-1.2505694785059221e-05</v>
+      </c>
+      <c r="M11" s="0">
         <v>2</v>
       </c>
-      <c r="L6" s="0">
+      <c r="N11" s="0">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="0">
+        <v>5</v>
+      </c>
+      <c r="D12" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="0">
+        <v>10</v>
+      </c>
+      <c r="F12" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G12" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H12" s="0">
+        <v>10</v>
+      </c>
+      <c r="I12" s="0">
+        <v>269</v>
+      </c>
+      <c r="J12" s="0">
+        <v>445.73144100000002</v>
+      </c>
+      <c r="K12" s="0">
+        <v>9.0414074238598374e-05</v>
+      </c>
+      <c r="L12" s="0">
+        <v>-2.2428847742544057e-05</v>
+      </c>
+      <c r="M12" s="0">
+        <v>2</v>
+      </c>
+      <c r="N12" s="0">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="0">
+        <v>5</v>
+      </c>
+      <c r="D13" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="0">
+        <v>10</v>
+      </c>
+      <c r="F13" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H13" s="0">
+        <v>10</v>
+      </c>
+      <c r="I13" s="0">
+        <v>270</v>
+      </c>
+      <c r="J13" s="0">
+        <v>257.27560979999998</v>
+      </c>
+      <c r="K13" s="0">
+        <v>0.00015197332929051122</v>
+      </c>
+      <c r="L13" s="0">
+        <v>-1.3869979997114833e-05</v>
+      </c>
+      <c r="M13" s="0">
+        <v>2</v>
+      </c>
+      <c r="N13" s="0">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>10</v>
+      </c>
+      <c r="B14" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="0">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E14" s="0">
+        <v>10</v>
+      </c>
+      <c r="F14" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H14" s="0">
+        <v>10</v>
+      </c>
+      <c r="I14" s="0">
+        <v>209</v>
+      </c>
+      <c r="J14" s="0">
+        <v>16.840199900000002</v>
+      </c>
+      <c r="K14" s="0">
+        <v>6.8850238741369196e-06</v>
+      </c>
+      <c r="L14" s="0">
+        <v>5.7037244069216536e-08</v>
+      </c>
+      <c r="M14" s="0">
+        <v>0</v>
+      </c>
+      <c r="N14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="0">
+        <v>5</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="0">
+        <v>10</v>
+      </c>
+      <c r="F15" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H15" s="0">
+        <v>10</v>
+      </c>
+      <c r="I15" s="0">
+        <v>269</v>
+      </c>
+      <c r="J15" s="0">
+        <v>123.6197784</v>
+      </c>
+      <c r="K15" s="0">
+        <v>7.1573757296494733e-06</v>
+      </c>
+      <c r="L15" s="0">
+        <v>5.8150525727170281e-08</v>
+      </c>
+      <c r="M15" s="0">
+        <v>0</v>
+      </c>
+      <c r="N15" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>10</v>
+      </c>
+      <c r="B16" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="0">
+        <v>5</v>
+      </c>
+      <c r="D16" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E16" s="0">
+        <v>10</v>
+      </c>
+      <c r="F16" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G16" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H16" s="0">
+        <v>10</v>
+      </c>
+      <c r="I16" s="0">
+        <v>251</v>
+      </c>
+      <c r="J16" s="0">
+        <v>120.6756374</v>
+      </c>
+      <c r="K16" s="0">
+        <v>9.4929486326389423e-05</v>
+      </c>
+      <c r="L16" s="0">
+        <v>-1.8186304555732276e-05</v>
+      </c>
+      <c r="M16" s="0">
+        <v>1</v>
+      </c>
+      <c r="N16" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>10</v>
+      </c>
+      <c r="B17" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="0">
+        <v>5</v>
+      </c>
+      <c r="D17" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="0">
+        <v>10</v>
+      </c>
+      <c r="F17" s="0">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H17" s="0">
+        <v>10</v>
+      </c>
+      <c r="I17" s="0">
+        <v>269</v>
+      </c>
+      <c r="J17" s="0">
+        <v>243.72695870000001</v>
+      </c>
+      <c r="K17" s="0">
+        <v>7.5919017148429191e-05</v>
+      </c>
+      <c r="L17" s="0">
+        <v>-1.2505694785059221e-05</v>
+      </c>
+      <c r="M17" s="0">
+        <v>2</v>
+      </c>
+      <c r="N17" s="0">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Generated all the base plots with noise.
</commit_message>
<xml_diff>
--- a/src/output/opt/noise/data.xlsx
+++ b/src/output/opt/noise/data.xlsx
@@ -69,8 +69,8 @@
     <col min="8" max="8" width="3" customWidth="true"/>
     <col min="9" max="9" width="5" customWidth="true"/>
     <col min="10" max="10" width="11.5546875" customWidth="true"/>
-    <col min="11" max="11" width="15.5546875" customWidth="true"/>
-    <col min="12" max="12" width="15.88671875" customWidth="true"/>
+    <col min="11" max="11" width="14.5546875" customWidth="true"/>
+    <col min="12" max="12" width="15.5546875" customWidth="true"/>
     <col min="13" max="13" width="2" customWidth="true"/>
     <col min="14" max="14" width="4" customWidth="true"/>
   </cols>
@@ -101,16 +101,16 @@
         <v>10</v>
       </c>
       <c r="I1" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J1" s="0">
-        <v>37.592995899999998</v>
+        <v>89.243538400000006</v>
       </c>
       <c r="K1" s="0">
-        <v>6.4932694991970408e-06</v>
+        <v>0.0011452752026068769</v>
       </c>
       <c r="L1" s="0">
-        <v>8.0009670018521097e-08</v>
+        <v>0.00017670182326759047</v>
       </c>
       <c r="M1" s="0">
         <v>0</v>
@@ -145,16 +145,16 @@
         <v>10</v>
       </c>
       <c r="I2" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="J2" s="0">
-        <v>93.003292599999995</v>
+        <v>198.4210301</v>
       </c>
       <c r="K2" s="0">
-        <v>7.2171191389802658e-06</v>
+        <v>0.0013440120782932663</v>
       </c>
       <c r="L2" s="0">
-        <v>6.287673443285553e-08</v>
+        <v>0.00018336590789271059</v>
       </c>
       <c r="M2" s="0">
         <v>0</v>
@@ -189,16 +189,16 @@
         <v>10</v>
       </c>
       <c r="I3" s="0">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="J3" s="0">
-        <v>100.07330109999999</v>
+        <v>241.57603230000001</v>
       </c>
       <c r="K3" s="0">
-        <v>7.1573757296494733e-06</v>
+        <v>0.0012797381774800609</v>
       </c>
       <c r="L3" s="0">
-        <v>5.8150525727170281e-08</v>
+        <v>0.0001934054255676059</v>
       </c>
       <c r="M3" s="0">
         <v>0</v>
@@ -233,16 +233,16 @@
         <v>10</v>
       </c>
       <c r="I4" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J4" s="0">
-        <v>130.79598559999999</v>
+        <v>285.82469040000001</v>
       </c>
       <c r="K4" s="0">
-        <v>6.4342353602864222e-06</v>
+        <v>0.001428688523450905</v>
       </c>
       <c r="L4" s="0">
-        <v>8.4126528430352524e-08</v>
+        <v>0.00020959038114722305</v>
       </c>
       <c r="M4" s="0">
         <v>0</v>
@@ -277,16 +277,16 @@
         <v>10</v>
       </c>
       <c r="I5" s="0">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J5" s="0">
-        <v>100.3150967</v>
+        <v>189.54301290000001</v>
       </c>
       <c r="K5" s="0">
-        <v>7.2719002239818309e-06</v>
+        <v>0.0016855521033674048</v>
       </c>
       <c r="L5" s="0">
-        <v>3.4547054183295656e-08</v>
+        <v>0.00019848763714879484</v>
       </c>
       <c r="M5" s="0">
         <v>1</v>
@@ -321,16 +321,16 @@
         <v>10</v>
       </c>
       <c r="I6" s="0">
-        <v>779</v>
+        <v>788</v>
       </c>
       <c r="J6" s="0">
-        <v>420.76224239999999</v>
+        <v>809.55318469999997</v>
       </c>
       <c r="K6" s="0">
-        <v>7.3346758511227961e-06</v>
+        <v>0.00156134978185829</v>
       </c>
       <c r="L6" s="0">
-        <v>1.0632717650283736e-08</v>
+        <v>0.00020824307857343987</v>
       </c>
       <c r="M6" s="0">
         <v>0</v>
@@ -365,16 +365,16 @@
         <v>10</v>
       </c>
       <c r="I7" s="0">
-        <v>1262</v>
+        <v>1286</v>
       </c>
       <c r="J7" s="0">
-        <v>436.4591729</v>
+        <v>1712.7446198</v>
       </c>
       <c r="K7" s="0">
-        <v>1.7145014564734495e-05</v>
+        <v>0.0018178502689683018</v>
       </c>
       <c r="L7" s="0">
-        <v>-1.3758434871880631e-07</v>
+        <v>0.0001805025436016349</v>
       </c>
       <c r="M7" s="0">
         <v>0</v>
@@ -409,22 +409,22 @@
         <v>10</v>
       </c>
       <c r="I8" s="0">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="J8" s="0">
-        <v>108.8751674</v>
+        <v>215.7881635</v>
       </c>
       <c r="K8" s="0">
-        <v>7.287129319077934e-06</v>
+        <v>0.0012400114727397771</v>
       </c>
       <c r="L8" s="0">
-        <v>5.0733148107113003e-08</v>
+        <v>0.00022390849220586047</v>
       </c>
       <c r="M8" s="0">
         <v>1</v>
       </c>
       <c r="N8" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -453,22 +453,22 @@
         <v>10</v>
       </c>
       <c r="I9" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="J9" s="0">
-        <v>119.39946329999999</v>
+        <v>234.1855151</v>
       </c>
       <c r="K9" s="0">
-        <v>2.7864391593190874e-05</v>
+        <v>0.0013339202775304315</v>
       </c>
       <c r="L9" s="0">
-        <v>3.6311749339572998e-08</v>
+        <v>0.00017829159837615108</v>
       </c>
       <c r="M9" s="0">
         <v>1</v>
       </c>
       <c r="N9" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
@@ -497,22 +497,22 @@
         <v>10</v>
       </c>
       <c r="I10" s="0">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="J10" s="0">
-        <v>228.01029969999999</v>
+        <v>817.5757691</v>
       </c>
       <c r="K10" s="0">
-        <v>2.7973201768949352e-05</v>
+        <v>0.0011519689145058631</v>
       </c>
       <c r="L10" s="0">
-        <v>-7.973671549211776e-07</v>
+        <v>0.00020460594234797855</v>
       </c>
       <c r="M10" s="0">
         <v>1</v>
       </c>
       <c r="N10" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -541,16 +541,16 @@
         <v>10</v>
       </c>
       <c r="I11" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="J11" s="0">
-        <v>231.72164889999999</v>
+        <v>323.64125680000001</v>
       </c>
       <c r="K11" s="0">
-        <v>7.5919017148429191e-05</v>
+        <v>0.0014627231347541514</v>
       </c>
       <c r="L11" s="0">
-        <v>-1.2505694785059221e-05</v>
+        <v>0.00017274467533679911</v>
       </c>
       <c r="M11" s="0">
         <v>2</v>
@@ -585,16 +585,16 @@
         <v>10</v>
       </c>
       <c r="I12" s="0">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="J12" s="0">
-        <v>445.73144100000002</v>
+        <v>313.73481399999997</v>
       </c>
       <c r="K12" s="0">
-        <v>9.0414074238598374e-05</v>
+        <v>0.0013883434331662947</v>
       </c>
       <c r="L12" s="0">
-        <v>-2.2428847742544057e-05</v>
+        <v>0.0001514347763090829</v>
       </c>
       <c r="M12" s="0">
         <v>2</v>
@@ -629,16 +629,16 @@
         <v>10</v>
       </c>
       <c r="I13" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="J13" s="0">
-        <v>257.27560979999998</v>
+        <v>472.09343189999998</v>
       </c>
       <c r="K13" s="0">
-        <v>0.00015197332929051122</v>
+        <v>0.0014953237659585117</v>
       </c>
       <c r="L13" s="0">
-        <v>-1.3869979997114833e-05</v>
+        <v>0.00017036604357627353</v>
       </c>
       <c r="M13" s="0">
         <v>2</v>

</xml_diff>